<commit_message>
nu realty data partial
</commit_message>
<xml_diff>
--- a/_files/person_natural_penading_raw_data.xlsx
+++ b/_files/person_natural_penading_raw_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\leon\projects\adin_2022\_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\leon\projects\adin_2022\_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AABE5BC-18C2-4395-B8C7-FE0D8C483625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0143E7-51E1-4B9D-A82A-62A83FAFA5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="7870" windowWidth="13970" windowHeight="20760" xr2:uid="{9DEB0A75-8ED5-4F71-9B73-776A3ED08638}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DEB0A75-8ED5-4F71-9B73-776A3ED08638}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>K55-13-44-A203</t>
   </si>
   <si>
-    <t>+572 6630509</t>
-  </si>
-  <si>
     <t>+57 3146327654</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>Mariela</t>
   </si>
   <si>
-    <t>+572 3966729</t>
-  </si>
-  <si>
     <t>A3-19-36</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>K29A-29-89</t>
   </si>
   <si>
-    <t>+57 23341781</t>
-  </si>
-  <si>
     <t>elizabeth-jaimes@hotmail.com</t>
   </si>
   <si>
@@ -545,6 +536,15 @@
   </si>
   <si>
     <t>K2N-18A-40-A5</t>
+  </si>
+  <si>
+    <t>+57 602 3966729</t>
+  </si>
+  <si>
+    <t>+57 602 6630509</t>
+  </si>
+  <si>
+    <t>+57 602 3341781</t>
   </si>
 </sst>
 </file>
@@ -900,24 +900,24 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:I33"/>
+      <selection activeCell="E2" activeCellId="1" sqref="A2:A33 E2:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -952,7 +952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14838593</v>
       </c>
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1130637949</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>352403</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31269983</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>31909009</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16792693</v>
       </c>
@@ -1144,13 +1144,13 @@
         <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>38963303</v>
       </c>
@@ -1158,13 +1158,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>168</v>
       </c>
       <c r="F8" t="s">
         <v>40</v>
@@ -1179,13 +1179,13 @@
         <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14639099</v>
       </c>
@@ -1193,13 +1193,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -1214,13 +1214,13 @@
         <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>31214798</v>
       </c>
@@ -1228,31 +1228,31 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
         <v>52</v>
-      </c>
-      <c r="G10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>31905442</v>
       </c>
@@ -1260,20 +1260,20 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" t="s">
         <v>57</v>
       </c>
-      <c r="F11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" t="s">
-        <v>59</v>
-      </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
@@ -1281,13 +1281,13 @@
         <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1114728401</v>
       </c>
@@ -1295,19 +1295,19 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" t="s">
-        <v>63</v>
-      </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
@@ -1316,13 +1316,13 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16300014</v>
       </c>
@@ -1330,34 +1330,34 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
         <v>65</v>
       </c>
-      <c r="G13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>67</v>
-      </c>
-      <c r="J13" t="s">
-        <v>69</v>
       </c>
       <c r="K13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>29185053</v>
       </c>
@@ -1365,34 +1365,34 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
         <v>72</v>
-      </c>
-      <c r="G14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" t="s">
-        <v>74</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>29185047</v>
       </c>
@@ -1400,20 +1400,20 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" t="s">
         <v>79</v>
       </c>
-      <c r="D15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" t="s">
-        <v>81</v>
-      </c>
       <c r="H15" t="s">
         <v>21</v>
       </c>
@@ -1421,13 +1421,13 @@
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>66818737</v>
       </c>
@@ -1435,19 +1435,19 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>66858587</v>
       </c>
@@ -1455,19 +1455,19 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1125230924</v>
       </c>
@@ -1475,19 +1475,19 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
         <v>21</v>
@@ -1496,13 +1496,13 @@
         <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>66904044</v>
       </c>
@@ -1510,34 +1510,34 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
         <v>89</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
         <v>90</v>
-      </c>
-      <c r="G19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" t="s">
-        <v>92</v>
       </c>
       <c r="K19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>80817426</v>
       </c>
@@ -1545,20 +1545,20 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" t="s">
         <v>101</v>
       </c>
-      <c r="F20" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" t="s">
-        <v>103</v>
-      </c>
       <c r="H20" t="s">
         <v>21</v>
       </c>
@@ -1566,13 +1566,13 @@
         <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17144443</v>
       </c>
@@ -1580,19 +1580,19 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" t="s">
-        <v>107</v>
-      </c>
       <c r="G21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H21" t="s">
         <v>21</v>
@@ -1601,13 +1601,13 @@
         <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>79052475</v>
       </c>
@@ -1615,20 +1615,20 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" t="s">
         <v>109</v>
       </c>
-      <c r="F22" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" t="s">
-        <v>111</v>
-      </c>
       <c r="H22" t="s">
         <v>21</v>
       </c>
@@ -1636,13 +1636,13 @@
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>41715862</v>
       </c>
@@ -1650,34 +1650,34 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" t="s">
         <v>116</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" t="s">
         <v>117</v>
       </c>
-      <c r="G23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" t="s">
-        <v>120</v>
-      </c>
-      <c r="I23" t="s">
-        <v>119</v>
-      </c>
       <c r="J23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16845080</v>
       </c>
@@ -1685,19 +1685,19 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H24" t="s">
         <v>21</v>
@@ -1706,13 +1706,13 @@
         <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13957385</v>
       </c>
@@ -1720,34 +1720,34 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" t="s">
         <v>128</v>
-      </c>
-      <c r="D25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" t="s">
-        <v>124</v>
-      </c>
-      <c r="G25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" t="s">
-        <v>130</v>
       </c>
       <c r="K25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>31233821</v>
       </c>
@@ -1755,16 +1755,16 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="G26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H26" t="s">
         <v>21</v>
@@ -1773,13 +1773,13 @@
         <v>19</v>
       </c>
       <c r="J26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>31248519</v>
       </c>
@@ -1787,16 +1787,16 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="G27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H27" t="s">
         <v>21</v>
@@ -1805,13 +1805,13 @@
         <v>19</v>
       </c>
       <c r="J27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>94041536</v>
       </c>
@@ -1819,19 +1819,19 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F28" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G28" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H28" t="s">
         <v>21</v>
@@ -1840,13 +1840,13 @@
         <v>19</v>
       </c>
       <c r="J28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>16678074</v>
       </c>
@@ -1854,31 +1854,31 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G29" t="s">
+        <v>155</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" t="s">
         <v>154</v>
       </c>
-      <c r="D29" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G29" t="s">
-        <v>158</v>
-      </c>
-      <c r="H29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I29" t="s">
-        <v>157</v>
-      </c>
       <c r="J29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>37275424</v>
       </c>
@@ -1886,31 +1886,31 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F30" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I30" t="s">
         <v>140</v>
       </c>
-      <c r="G30" t="s">
+      <c r="J30" t="s">
         <v>141</v>
-      </c>
-      <c r="I30" t="s">
-        <v>143</v>
-      </c>
-      <c r="J30" t="s">
-        <v>144</v>
       </c>
       <c r="K30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>88233076</v>
       </c>
@@ -1918,31 +1918,31 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G31" t="s">
+        <v>138</v>
+      </c>
+      <c r="I31" t="s">
+        <v>140</v>
+      </c>
+      <c r="J31" t="s">
         <v>141</v>
-      </c>
-      <c r="I31" t="s">
-        <v>143</v>
-      </c>
-      <c r="J31" t="s">
-        <v>144</v>
       </c>
       <c r="K31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1130668637</v>
       </c>
@@ -1950,20 +1950,20 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F32" t="s">
+        <v>161</v>
+      </c>
+      <c r="G32" t="s">
         <v>160</v>
       </c>
-      <c r="D32" t="s">
-        <v>161</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" t="s">
-        <v>164</v>
-      </c>
-      <c r="G32" t="s">
-        <v>163</v>
-      </c>
       <c r="H32" t="s">
         <v>21</v>
       </c>
@@ -1971,13 +1971,13 @@
         <v>19</v>
       </c>
       <c r="J32" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>52818113</v>
       </c>
@@ -1985,20 +1985,20 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" t="s">
         <v>165</v>
       </c>
-      <c r="D33" t="s">
+      <c r="G33" t="s">
         <v>166</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F33" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33" t="s">
-        <v>169</v>
-      </c>
       <c r="H33" t="s">
         <v>21</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>19</v>
       </c>
       <c r="J33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K33">
         <v>2</v>

</xml_diff>

<commit_message>
nu address data partial
</commit_message>
<xml_diff>
--- a/_files/person_natural_penading_raw_data.xlsx
+++ b/_files/person_natural_penading_raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\leon\projects\adin_2022\_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0143E7-51E1-4B9D-A82A-62A83FAFA5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D839D4D9-C385-469D-96D6-23A7A7E43FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DEB0A75-8ED5-4F71-9B73-776A3ED08638}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="171">
   <si>
     <t>id_number</t>
   </si>
@@ -127,18 +127,6 @@
     <t>Jaramillo Ospina</t>
   </si>
   <si>
-    <t>+1 7543045130</t>
-  </si>
-  <si>
-    <t>+57 3164071898</t>
-  </si>
-  <si>
-    <t>+57 3166841377</t>
-  </si>
-  <si>
-    <t>+1 8045546462</t>
-  </si>
-  <si>
     <t>rociojaramillo@aol.com</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
     <t>Velez</t>
   </si>
   <si>
-    <t>+57 3156074411</t>
-  </si>
-  <si>
     <t>juan.carlos.velez@correounivalle.edu.co</t>
   </si>
   <si>
@@ -166,9 +151,6 @@
     <t>K55-13-44-A203</t>
   </si>
   <si>
-    <t>+57 3146327654</t>
-  </si>
-  <si>
     <t>A6N-13N-62-S111^2022-07-01</t>
   </si>
   <si>
@@ -202,9 +184,6 @@
     <t>Tenorio Rojas</t>
   </si>
   <si>
-    <t>+57 3186490366</t>
-  </si>
-  <si>
     <t>vmack02@hotmail.com</t>
   </si>
   <si>
@@ -217,15 +196,9 @@
     <t>Oca Motato</t>
   </si>
   <si>
-    <t>+57 3168703511</t>
-  </si>
-  <si>
     <t>danita465@hotmail.com</t>
   </si>
   <si>
-    <t>+57 3106431401</t>
-  </si>
-  <si>
     <t>stevenmorajimenez@outlook.com</t>
   </si>
   <si>
@@ -262,18 +235,12 @@
     <t>Estacio Osorio</t>
   </si>
   <si>
-    <t>+57 3178002340</t>
-  </si>
-  <si>
     <t>C3-8-49</t>
   </si>
   <si>
     <t>Nelly Amparo</t>
   </si>
   <si>
-    <t>+57 3154630661</t>
-  </si>
-  <si>
     <t>C62b-3-90</t>
   </si>
   <si>
@@ -298,9 +265,6 @@
     <t>C17N-9-90</t>
   </si>
   <si>
-    <t>+57 3168712962</t>
-  </si>
-  <si>
     <t>moni3074@hotmail.com</t>
   </si>
   <si>
@@ -325,18 +289,12 @@
     <t>A6N-13N-62-S318^2021-08-01</t>
   </si>
   <si>
-    <t>+57 3174899555</t>
-  </si>
-  <si>
     <t>Alejandro</t>
   </si>
   <si>
     <t>Dominguez Cabal</t>
   </si>
   <si>
-    <t>+57 3166418549</t>
-  </si>
-  <si>
     <t>alejosunday@gmail.com</t>
   </si>
   <si>
@@ -349,18 +307,12 @@
     <t>Dominguez Plaza</t>
   </si>
   <si>
-    <t>+57 3174286020</t>
-  </si>
-  <si>
     <t>alfonsodominguezp@hotmail.com</t>
   </si>
   <si>
     <t>A6N-13N-62-S319^2021-08-01</t>
   </si>
   <si>
-    <t>+57 3165551566</t>
-  </si>
-  <si>
     <t>miguelbuitragop@gmail.com</t>
   </si>
   <si>
@@ -379,9 +331,6 @@
     <t>Moreno Sarmiento</t>
   </si>
   <si>
-    <t>+57 3118209865</t>
-  </si>
-  <si>
     <t>jenny611@gmail.com</t>
   </si>
   <si>
@@ -394,15 +343,9 @@
     <t>Cundinamarca</t>
   </si>
   <si>
-    <t>+57 31040882215</t>
-  </si>
-  <si>
     <t>hedatolo@gmail.com</t>
   </si>
   <si>
-    <t>+57 3012541700</t>
-  </si>
-  <si>
     <t>edgar.perez0509@gmail.com</t>
   </si>
   <si>
@@ -469,21 +412,12 @@
     <t>Jaimes Suarez</t>
   </si>
   <si>
-    <t>+57 3208961514</t>
-  </si>
-  <si>
     <t>Gerson Alexander</t>
   </si>
   <si>
     <t>Urbina</t>
   </si>
   <si>
-    <t>+57 3156389025</t>
-  </si>
-  <si>
-    <t>+57 3164186372</t>
-  </si>
-  <si>
     <t>roca191@hotmail.com</t>
   </si>
   <si>
@@ -496,9 +430,6 @@
     <t>Castro Gomez</t>
   </si>
   <si>
-    <t>*57 3128696103</t>
-  </si>
-  <si>
     <t>Candelaria</t>
   </si>
   <si>
@@ -514,9 +445,6 @@
     <t>Osorio Salazar</t>
   </si>
   <si>
-    <t>+57 3006087604</t>
-  </si>
-  <si>
     <t>A9AN-10N-76</t>
   </si>
   <si>
@@ -529,9 +457,6 @@
     <t>Osorio Marquez</t>
   </si>
   <si>
-    <t>+57 3006087520</t>
-  </si>
-  <si>
     <t>om.andrea@gmail.com</t>
   </si>
   <si>
@@ -545,6 +470,84 @@
   </si>
   <si>
     <t>+57 602 3341781</t>
+  </si>
+  <si>
+    <t>+57 316 4071898</t>
+  </si>
+  <si>
+    <t>+57 316 6841377</t>
+  </si>
+  <si>
+    <t>+1 754 3045130</t>
+  </si>
+  <si>
+    <t>+1 804 5546462</t>
+  </si>
+  <si>
+    <t>+57 315 6074411</t>
+  </si>
+  <si>
+    <t>+57 314 6327654</t>
+  </si>
+  <si>
+    <t>+57 318 6490366</t>
+  </si>
+  <si>
+    <t>+57 316 8703511</t>
+  </si>
+  <si>
+    <t>+57 310 6431401</t>
+  </si>
+  <si>
+    <t>+57 317 8002340</t>
+  </si>
+  <si>
+    <t>+57 315 4630661</t>
+  </si>
+  <si>
+    <t>+57 317 4899555</t>
+  </si>
+  <si>
+    <t>+57 316 8712962</t>
+  </si>
+  <si>
+    <t>+57 316 6418549</t>
+  </si>
+  <si>
+    <t>+57 317 4286020</t>
+  </si>
+  <si>
+    <t>+57 316 5551566</t>
+  </si>
+  <si>
+    <t>+57 311 8209865</t>
+  </si>
+  <si>
+    <t>+57 310 40882215</t>
+  </si>
+  <si>
+    <t>+57 301 2541700</t>
+  </si>
+  <si>
+    <t>+57 316 4186372</t>
+  </si>
+  <si>
+    <t>*57 312 8696103</t>
+  </si>
+  <si>
+    <t>+57 320 8961514</t>
+  </si>
+  <si>
+    <t>+57 315 6389025</t>
+  </si>
+  <si>
+    <t>+57 300 6087604</t>
+  </si>
+  <si>
+    <t>+57 300 6087520</t>
+  </si>
+  <si>
+    <t>Santander</t>
   </si>
 </sst>
 </file>
@@ -900,7 +903,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="A2:A33 E2:E33"/>
+      <selection activeCell="H6" sqref="H6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -1001,7 +1004,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -1036,7 +1039,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -1068,7 +1071,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>33</v>
+        <v>148</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
@@ -1094,10 +1097,10 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" t="s">
         <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -1123,28 +1126,28 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
         <v>38</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>44</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1158,19 +1161,19 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
@@ -1179,7 +1182,7 @@
         <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -1193,19 +1196,19 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
@@ -1214,7 +1217,7 @@
         <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -1228,16 +1231,16 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
@@ -1246,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1260,19 +1263,19 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
@@ -1281,7 +1284,7 @@
         <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -1295,28 +1298,28 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" t="s">
-        <v>67</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1330,28 +1333,28 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
         <v>21</v>
       </c>
       <c r="I13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -1365,19 +1368,19 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
         <v>21</v>
@@ -1386,7 +1389,7 @@
         <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1400,19 +1403,19 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H15" t="s">
         <v>21</v>
@@ -1421,7 +1424,7 @@
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="K15">
         <v>2</v>
@@ -1435,13 +1438,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1455,13 +1458,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="K17">
         <v>2</v>
@@ -1475,19 +1478,19 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
         <v>21</v>
@@ -1496,7 +1499,7 @@
         <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1510,19 +1513,19 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
         <v>21</v>
@@ -1531,7 +1534,7 @@
         <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="K19">
         <v>2</v>
@@ -1545,19 +1548,19 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s">
         <v>21</v>
@@ -1566,7 +1569,7 @@
         <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -1580,19 +1583,19 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G21" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H21" t="s">
         <v>21</v>
@@ -1601,7 +1604,7 @@
         <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -1615,19 +1618,19 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="H22" t="s">
         <v>21</v>
@@ -1636,7 +1639,7 @@
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -1650,28 +1653,28 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="F23" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="G23" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="H23" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="I23" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="J23" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K23">
         <v>2</v>
@@ -1685,19 +1688,19 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="F24" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="G24" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="H24" t="s">
         <v>21</v>
@@ -1706,7 +1709,7 @@
         <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -1720,19 +1723,19 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="F25" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="G25" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="H25" t="s">
         <v>21</v>
@@ -1741,7 +1744,7 @@
         <v>19</v>
       </c>
       <c r="J25" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="K25">
         <v>2</v>
@@ -1755,16 +1758,16 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="G26" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
         <v>21</v>
@@ -1773,7 +1776,7 @@
         <v>19</v>
       </c>
       <c r="J26" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -1787,16 +1790,16 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="G27" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="H27" t="s">
         <v>21</v>
@@ -1805,7 +1808,7 @@
         <v>19</v>
       </c>
       <c r="J27" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="K27">
         <v>2</v>
@@ -1819,19 +1822,19 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="F28" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="G28" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="H28" t="s">
         <v>21</v>
@@ -1840,7 +1843,7 @@
         <v>19</v>
       </c>
       <c r="J28" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -1854,25 +1857,25 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="G29" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="H29" t="s">
         <v>21</v>
       </c>
       <c r="I29" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="J29" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="K29">
         <v>2</v>
@@ -1886,25 +1889,28 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="G30" t="s">
-        <v>138</v>
+        <v>119</v>
+      </c>
+      <c r="H30" t="s">
+        <v>170</v>
       </c>
       <c r="I30" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="J30" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -1918,25 +1924,28 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="G31" t="s">
-        <v>138</v>
+        <v>119</v>
+      </c>
+      <c r="H31" t="s">
+        <v>170</v>
       </c>
       <c r="I31" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="J31" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="K31">
         <v>2</v>
@@ -1950,19 +1959,19 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="G32" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="H32" t="s">
         <v>21</v>
@@ -1971,7 +1980,7 @@
         <v>19</v>
       </c>
       <c r="J32" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -1985,19 +1994,19 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="G33" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="H33" t="s">
         <v>21</v>
@@ -2006,7 +2015,7 @@
         <v>19</v>
       </c>
       <c r="J33" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="K33">
         <v>2</v>

</xml_diff>

<commit_message>
nu people data partial
</commit_message>
<xml_diff>
--- a/_files/person_natural_penading_raw_data.xlsx
+++ b/_files/person_natural_penading_raw_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\leon\projects\adin_2022\_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\leon\projects\adin_2022\_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D839D4D9-C385-469D-96D6-23A7A7E43FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC06BB-F936-4F6C-AA35-BA0692D6B060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DEB0A75-8ED5-4F71-9B73-776A3ED08638}"/>
+    <workbookView xWindow="-5790" yWindow="6980" windowWidth="13970" windowHeight="20760" xr2:uid="{9DEB0A75-8ED5-4F71-9B73-776A3ED08638}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="180">
   <si>
     <t>id_number</t>
   </si>
@@ -548,6 +548,33 @@
   </si>
   <si>
     <t>Santander</t>
+  </si>
+  <si>
+    <t>+57 316 4788629</t>
+  </si>
+  <si>
+    <t>adriabego@yahoo.es</t>
+  </si>
+  <si>
+    <t>C13-9-36</t>
+  </si>
+  <si>
+    <t>+57 304 5235781</t>
+  </si>
+  <si>
+    <t>sicolog@hotmail.com</t>
+  </si>
+  <si>
+    <t>C4S-48-10-A603</t>
+  </si>
+  <si>
+    <t>Villa del Rosario</t>
+  </si>
+  <si>
+    <t>Santa Ana</t>
+  </si>
+  <si>
+    <t>Metropolitano Norte</t>
   </si>
 </sst>
 </file>
@@ -900,27 +927,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC96F5A-27CD-49B1-92F6-8C43E5CD171F}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:I6"/>
+      <selection activeCell="G16" sqref="G16:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="8.1796875" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>14838593</v>
       </c>
@@ -990,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1130637949</v>
       </c>
@@ -1025,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>352403</v>
       </c>
@@ -1057,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>31269983</v>
       </c>
@@ -1083,7 +1110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>31909009</v>
       </c>
@@ -1118,7 +1145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16792693</v>
       </c>
@@ -1153,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>38963303</v>
       </c>
@@ -1188,7 +1215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>14639099</v>
       </c>
@@ -1223,7 +1250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>31214798</v>
       </c>
@@ -1255,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>31905442</v>
       </c>
@@ -1290,7 +1317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1114728401</v>
       </c>
@@ -1325,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>16300014</v>
       </c>
@@ -1360,7 +1387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>29185053</v>
       </c>
@@ -1395,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>29185047</v>
       </c>
@@ -1430,7 +1457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>66818737</v>
       </c>
@@ -1443,6 +1470,21 @@
       <c r="D16" t="s">
         <v>71</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" t="s">
+        <v>172</v>
+      </c>
+      <c r="G16" t="s">
+        <v>173</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
       <c r="J16" t="s">
         <v>69</v>
       </c>
@@ -1450,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>66858587</v>
       </c>
@@ -1463,6 +1505,21 @@
       <c r="D17" t="s">
         <v>73</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
       <c r="J17" t="s">
         <v>69</v>
       </c>
@@ -1470,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1125230924</v>
       </c>
@@ -1505,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>66904044</v>
       </c>
@@ -1540,7 +1597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>80817426</v>
       </c>
@@ -1575,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>17144443</v>
       </c>
@@ -1610,7 +1667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>79052475</v>
       </c>
@@ -1645,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>41715862</v>
       </c>
@@ -1680,7 +1737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>16845080</v>
       </c>
@@ -1715,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>13957385</v>
       </c>
@@ -1750,7 +1807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>31233821</v>
       </c>
@@ -1782,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>31248519</v>
       </c>
@@ -1814,7 +1871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>94041536</v>
       </c>
@@ -1848,8 +1905,11 @@
       <c r="K28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>16678074</v>
       </c>
@@ -1880,8 +1940,11 @@
       <c r="K29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>37275424</v>
       </c>
@@ -1915,8 +1978,11 @@
       <c r="K30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>88233076</v>
       </c>
@@ -1950,8 +2016,11 @@
       <c r="K31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1130668637</v>
       </c>
@@ -1986,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>52818113</v>
       </c>

</xml_diff>